<commit_message>
added all the assertions and extend report
</commit_message>
<xml_diff>
--- a/src/TestDataExcel.xlsx
+++ b/src/TestDataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PujaPowar\IdeaProjects\DataDrivenTestingFramework\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5661DB-1334-4BD0-ADD1-273F1081EFE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B63C66-AB7D-46C6-8023-C209695B50C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A58002A-2DAB-4554-9D92-048F153DD65F}"/>
   </bookViews>
@@ -458,7 +458,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,7 +482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
added scrolling and country selection code
</commit_message>
<xml_diff>
--- a/src/TestDataExcel.xlsx
+++ b/src/TestDataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PujaPowar\IdeaProjects\DataDrivenTestingFramework\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A2815C-CABC-4B23-B06B-8AB893465706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F184C33-DCD6-4FAB-A46D-8A28860D4FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A58002A-2DAB-4554-9D92-048F153DD65F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Environment</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Stage</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
   </si>
 </sst>
 </file>
@@ -473,7 +476,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,6 +484,7 @@
     <col min="1" max="1" width="12.109375" customWidth="1"/>
     <col min="2" max="2" width="29.21875" customWidth="1"/>
     <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
     <col min="5" max="5" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -499,18 +503,18 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -561,7 +565,7 @@
     <hyperlink ref="B11" r:id="rId1" xr:uid="{917FA582-DBEA-4641-84A6-0C1C3011CF03}"/>
     <hyperlink ref="B10" r:id="rId2" xr:uid="{C7B906C3-28CA-46C3-85FD-5068FF31BB08}"/>
     <hyperlink ref="B9" r:id="rId3" xr:uid="{1855214D-D692-4F60-B17C-CB234106C238}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{75C55A57-3645-4CA3-B751-1374A02FE9C2}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{408DF9C0-09E4-4CB9-A744-7AC5511797A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added user management code
</commit_message>
<xml_diff>
--- a/src/TestDataExcel.xlsx
+++ b/src/TestDataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PujaPowar\IdeaProjects\DataDrivenTestingFramework\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F184C33-DCD6-4FAB-A46D-8A28860D4FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5860B4B3-323A-4F43-8CE8-4FE10CC2F251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A58002A-2DAB-4554-9D92-048F153DD65F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Environment</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Stage</t>
-  </si>
-  <si>
-    <t>Netherlands</t>
   </si>
 </sst>
 </file>
@@ -476,7 +473,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -503,7 +500,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -514,7 +511,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -565,7 +562,7 @@
     <hyperlink ref="B11" r:id="rId1" xr:uid="{917FA582-DBEA-4641-84A6-0C1C3011CF03}"/>
     <hyperlink ref="B10" r:id="rId2" xr:uid="{C7B906C3-28CA-46C3-85FD-5068FF31BB08}"/>
     <hyperlink ref="B9" r:id="rId3" xr:uid="{1855214D-D692-4F60-B17C-CB234106C238}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{408DF9C0-09E4-4CB9-A744-7AC5511797A7}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{A80E5EF5-58F1-4748-8FB5-E5823D3AE747}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
this is user managment code
</commit_message>
<xml_diff>
--- a/src/TestDataExcel.xlsx
+++ b/src/TestDataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PujaPowar\IdeaProjects\DataDrivenTestingFramework\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5860B4B3-323A-4F43-8CE8-4FE10CC2F251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630D475C-ABAE-4C02-A124-3B1D0077D888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A58002A-2DAB-4554-9D92-048F153DD65F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Environment</t>
   </si>
@@ -72,6 +72,27 @@
   </si>
   <si>
     <t>Stage</t>
+  </si>
+  <si>
+    <t>email id</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>pujapowar@yopmail.com</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>Super Admin</t>
+  </si>
+  <si>
+    <t>tester</t>
   </si>
 </sst>
 </file>
@@ -124,7 +145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -135,6 +156,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -470,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F255A06-1447-4E91-95E4-88AFEF6A08E6}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,7 +507,7 @@
     <col min="5" max="5" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,23 +520,46 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -528,7 +573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -542,7 +587,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -562,7 +607,8 @@
     <hyperlink ref="B11" r:id="rId1" xr:uid="{917FA582-DBEA-4641-84A6-0C1C3011CF03}"/>
     <hyperlink ref="B10" r:id="rId2" xr:uid="{C7B906C3-28CA-46C3-85FD-5068FF31BB08}"/>
     <hyperlink ref="B9" r:id="rId3" xr:uid="{1855214D-D692-4F60-B17C-CB234106C238}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{A80E5EF5-58F1-4748-8FB5-E5823D3AE747}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{C59540FF-95F3-4CD6-AA1F-D4EA3D0E256C}"/>
+    <hyperlink ref="E2" r:id="rId5" xr:uid="{8B6E6A10-B32C-42E5-981F-824C45A30C82}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
completed user management screnrio
</commit_message>
<xml_diff>
--- a/src/TestDataExcel.xlsx
+++ b/src/TestDataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PujaPowar\IdeaProjects\DataDrivenTestingFramework\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1474094-AD5C-4826-A93A-65FBEC6B483A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9405944B-7B2F-46C9-B064-3E73AC039EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A58002A-2DAB-4554-9D92-048F153DD65F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>Environment</t>
   </si>
@@ -62,15 +62,9 @@
     <t>password</t>
   </si>
   <si>
-    <t>Romania</t>
-  </si>
-  <si>
     <t>Dev</t>
   </si>
   <si>
-    <t>n8cjtVdQgt</t>
-  </si>
-  <si>
     <t>Stage</t>
   </si>
   <si>
@@ -96,6 +90,9 @@
   </si>
   <si>
     <t>testing</t>
+  </si>
+  <si>
+    <t>Australia</t>
   </si>
 </sst>
 </file>
@@ -525,42 +522,42 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -574,50 +571,50 @@
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
         <v>17</v>
       </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" t="s">
-        <v>19</v>
-      </c>
       <c r="H9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" t="s">
-        <v>19</v>
-      </c>
       <c r="H10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
@@ -626,19 +623,19 @@
         <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" t="s">
-        <v>19</v>
-      </c>
       <c r="H11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -650,8 +647,8 @@
     <hyperlink ref="E9" r:id="rId4" xr:uid="{725A8482-E266-4366-9FF9-3CDDD7974C64}"/>
     <hyperlink ref="E10" r:id="rId5" xr:uid="{AF6B89B1-88BC-41BA-9546-400C280D696E}"/>
     <hyperlink ref="E11" r:id="rId6" xr:uid="{CF38D19E-7965-4709-842E-0B05A8933321}"/>
-    <hyperlink ref="B2" r:id="rId7" xr:uid="{B19980CB-85B8-410E-968D-D4630EB2B5EE}"/>
-    <hyperlink ref="E2" r:id="rId8" xr:uid="{B72D98A1-FEBF-4404-B6F0-BAA91D9517F1}"/>
+    <hyperlink ref="B2" r:id="rId7" xr:uid="{50442B45-148F-4507-9C9D-5E26693071BB}"/>
+    <hyperlink ref="E2" r:id="rId8" xr:uid="{4EB1939C-4728-4E3B-BED7-8F88232E39A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added validation code as komal told
</commit_message>
<xml_diff>
--- a/src/TestDataExcel.xlsx
+++ b/src/TestDataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PujaPowar\IdeaProjects\DataDrivenTestingFramework\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA935F42-BDFE-442C-8602-079DCAE07EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FA3454-CE59-45D1-8270-681192B92E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A58002A-2DAB-4554-9D92-048F153DD65F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>Environment</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Australia</t>
+  </si>
+  <si>
+    <t>Germany</t>
   </si>
 </sst>
 </file>
@@ -495,7 +498,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,7 +548,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
adding user management code
</commit_message>
<xml_diff>
--- a/src/TestDataExcel.xlsx
+++ b/src/TestDataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PujaPowar\IdeaProjects\DataDrivenTestingFramework\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FA3454-CE59-45D1-8270-681192B92E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45244258-9784-41FE-963D-C031AA81F0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A58002A-2DAB-4554-9D92-048F153DD65F}"/>
   </bookViews>
@@ -498,7 +498,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added new chrome version
</commit_message>
<xml_diff>
--- a/src/TestDataExcel.xlsx
+++ b/src/TestDataExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PIP Discussion\DataDrivenTestingFramework\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C937C4-0CC6-4FA9-944E-FF3D9B575666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7383D3B-4B83-4730-A17E-6318BC130BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A58002A-2DAB-4554-9D92-048F153DD65F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
   <si>
     <t>Environment</t>
   </si>
@@ -105,15 +105,6 @@
   </si>
   <si>
     <t>Prod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UY26o65m5H </t>
-  </si>
-  <si>
-    <t>puja.powar@cloverbaytechnologies.com</t>
-  </si>
-  <si>
-    <t>cbtestingteam@cloverbaytechnologies.com</t>
   </si>
 </sst>
 </file>
@@ -516,7 +507,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,21 +550,21 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>22</v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -709,8 +700,8 @@
     <hyperlink ref="B3" r:id="rId7" xr:uid="{AF29E4B2-C235-409D-BB5D-D87289BEDDAB}"/>
     <hyperlink ref="B12" r:id="rId8" xr:uid="{0B12E878-416D-42F8-B2C1-DC0698021D5F}"/>
     <hyperlink ref="E12" r:id="rId9" xr:uid="{A9ABFC17-1974-440F-B83D-5F05CE37DDC5}"/>
-    <hyperlink ref="B2" r:id="rId10" xr:uid="{66EDA9E6-3DA1-43D3-9623-88BBF973AD4F}"/>
-    <hyperlink ref="E2" r:id="rId11" xr:uid="{08D45E5E-C88A-475C-952C-717763DF8986}"/>
+    <hyperlink ref="B2" r:id="rId10" xr:uid="{5FB91629-F07D-4C8F-B6B8-D25FC6EA58D3}"/>
+    <hyperlink ref="E2" r:id="rId11" xr:uid="{A4235BCC-3914-4AF7-A675-D77228ACCA22}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>